<commit_message>
Adds final details to the ML models and to the tests
</commit_message>
<xml_diff>
--- a/TestsForNN.xlsx
+++ b/TestsForNN.xlsx
@@ -8,14 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\biaco\MEOCloud\UA\AA\Projeto\AA-Projeto1-main\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F83B2B58-88C0-4204-8715-8D6022FC50A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E338E283-EC30-4CBB-98B1-7B597A3A9134}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{4F881D6F-E29F-4FDB-B849-47811DDC3998}"/>
+    <workbookView xWindow="9195" yWindow="2460" windowWidth="18495" windowHeight="11385" activeTab="2" xr2:uid="{4F881D6F-E29F-4FDB-B849-47811DDC3998}"/>
   </bookViews>
   <sheets>
     <sheet name="1st Phase" sheetId="1" r:id="rId1"/>
     <sheet name="2nd Phase" sheetId="2" r:id="rId2"/>
     <sheet name="3rd Phase" sheetId="3" r:id="rId3"/>
+    <sheet name="4th Phase" sheetId="4" r:id="rId4"/>
+    <sheet name="LR" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="119">
   <si>
     <t>Training Set</t>
   </si>
@@ -235,6 +237,165 @@
   </si>
   <si>
     <t>https://imgur.com/a/XJzCdu7</t>
+  </si>
+  <si>
+    <t>4th Phase</t>
+  </si>
+  <si>
+    <t>#11</t>
+  </si>
+  <si>
+    <t>100x101</t>
+  </si>
+  <si>
+    <t>#12</t>
+  </si>
+  <si>
+    <t>100x102</t>
+  </si>
+  <si>
+    <t>https://imgur.com/a/Lkcypmi</t>
+  </si>
+  <si>
+    <t>https://imgur.com/a/RqILb6M</t>
+  </si>
+  <si>
+    <t>Validation Set</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Images Size </t>
+  </si>
+  <si>
+    <t>Images Size</t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t># Classes</t>
+  </si>
+  <si>
+    <t>Train Set</t>
+  </si>
+  <si>
+    <t>Num. Iters</t>
+  </si>
+  <si>
+    <t>Train Set Acc</t>
+  </si>
+  <si>
+    <t>Test Set Acc</t>
+  </si>
+  <si>
+    <t>https://imgur.com/a/4yb61Cx</t>
+  </si>
+  <si>
+    <t>https://imgur.com/a/ljKCGI4</t>
+  </si>
+  <si>
+    <t>https://imgur.com/a/4BXDJW3</t>
+  </si>
+  <si>
+    <t>https://imgur.com/a/bFmorLx</t>
+  </si>
+  <si>
+    <t>https://imgur.com/a/awaBu4X</t>
+  </si>
+  <si>
+    <t>https://imgur.com/a/7zSVIpl</t>
+  </si>
+  <si>
+    <t>Min CV Acc</t>
+  </si>
+  <si>
+    <t>Max CV Acc</t>
+  </si>
+  <si>
+    <t>76.791%/77.289%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Avg CV Acc </t>
+  </si>
+  <si>
+    <t>K-Fold vs Stratified</t>
+  </si>
+  <si>
+    <t>73.443%/73.858%</t>
+  </si>
+  <si>
+    <t>0.02938/ 0.02780</t>
+  </si>
+  <si>
+    <t>Std Deviation</t>
+  </si>
+  <si>
+    <t>0.02313/0.02788</t>
+  </si>
+  <si>
+    <t>81.042%/80.952%</t>
+  </si>
+  <si>
+    <t>74.761%/73.809%</t>
+  </si>
+  <si>
+    <t>78.039%/77.376%</t>
+  </si>
+  <si>
+    <t>Dev Set</t>
+  </si>
+  <si>
+    <t>/</t>
+  </si>
+  <si>
+    <t>0.03860/0.03155</t>
+  </si>
+  <si>
+    <t>80.663%/79.005%</t>
+  </si>
+  <si>
+    <t>76.133%/76.023%</t>
+  </si>
+  <si>
+    <t>https://imgur.com/a/UsnGGqW</t>
+  </si>
+  <si>
+    <t>https://imgur.com/a/VgMNRsY</t>
+  </si>
+  <si>
+    <t>73.919%/74.699%</t>
+  </si>
+  <si>
+    <t>72.375%/70.718%</t>
+  </si>
+  <si>
+    <t>75.555%/76.666%</t>
+  </si>
+  <si>
+    <t>0.01314/0.02467</t>
+  </si>
+  <si>
+    <t>https://imgur.com/a/u5xlYdN</t>
+  </si>
+  <si>
+    <t>https://imgur.com/a/nNAocXz</t>
+  </si>
+  <si>
+    <t>77.916%/79.166%</t>
+  </si>
+  <si>
+    <t>75.416%/76.25%</t>
+  </si>
+  <si>
+    <t>77.037%/77.371%</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.00965/0.01226</t>
+  </si>
+  <si>
+    <t>81.25%/81.25%</t>
+  </si>
+  <si>
+    <t>71.667%/ 71.111%</t>
   </si>
 </sst>
 </file>
@@ -242,9 +403,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.000%"/>
+    <numFmt numFmtId="164" formatCode="0.000%"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -290,6 +451,17 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial Unicode MS"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial Unicode MS"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -299,7 +471,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="24">
+  <borders count="44">
     <border>
       <left/>
       <right/>
@@ -626,6 +798,242 @@
       <right style="medium">
         <color indexed="64"/>
       </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top/>
       <bottom style="medium">
         <color indexed="64"/>
@@ -638,7 +1046,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="101">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -646,7 +1054,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -667,7 +1075,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -694,7 +1102,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="2" applyBorder="1" applyAlignment="1">
@@ -733,7 +1141,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="2" applyBorder="1" applyAlignment="1">
@@ -748,7 +1156,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -763,7 +1171,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -778,7 +1186,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="21" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -796,22 +1204,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
@@ -822,6 +1230,109 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="25" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="6" fillId="0" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1142,10 +1653,10 @@
   <dimension ref="A2:N22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I31" sqref="I31"/>
+      <selection activeCell="B6" sqref="B6:L14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.42578125" style="1" bestFit="1" customWidth="1"/>
@@ -1163,16 +1674,16 @@
     <col min="14" max="14" width="32.28515625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14">
       <c r="N2" s="7"/>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14">
       <c r="A3" s="6" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="6" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" ht="15.75" thickBot="1"/>
+    <row r="6" spans="1:14" ht="15.75" thickBot="1">
       <c r="B6" s="34" t="s">
         <v>8</v>
       </c>
@@ -1210,7 +1721,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14">
       <c r="B7" s="28" t="s">
         <v>9</v>
       </c>
@@ -1248,7 +1759,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" ht="18.75" customHeight="1">
       <c r="B8" s="12" t="s">
         <v>11</v>
       </c>
@@ -1286,7 +1797,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14">
       <c r="B9" s="12" t="s">
         <v>13</v>
       </c>
@@ -1324,7 +1835,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14">
       <c r="B10" s="12" t="s">
         <v>14</v>
       </c>
@@ -1362,7 +1873,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14">
       <c r="B11" s="12" t="s">
         <v>16</v>
       </c>
@@ -1400,7 +1911,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14">
       <c r="B12" s="12" t="s">
         <v>19</v>
       </c>
@@ -1438,7 +1949,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14">
       <c r="B13" s="12" t="s">
         <v>21</v>
       </c>
@@ -1476,7 +1987,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:14" ht="15.75" thickBot="1">
       <c r="B14" s="15" t="s">
         <v>23</v>
       </c>
@@ -1514,25 +2025,25 @@
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14">
       <c r="F16" s="1"/>
       <c r="G16" s="4"/>
       <c r="K16" s="1"/>
       <c r="M16" s="3"/>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13">
       <c r="F17" s="1"/>
       <c r="G17" s="4"/>
       <c r="K17" s="1"/>
       <c r="M17" s="3"/>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13">
       <c r="F18" s="1"/>
       <c r="G18" s="4"/>
       <c r="K18" s="1"/>
       <c r="M18" s="3"/>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13">
       <c r="A22" s="6"/>
     </row>
   </sheetData>
@@ -1553,50 +2064,51 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{632B25C1-EED0-43FB-9A19-E2017DDCB1BC}">
-  <dimension ref="A2:N15"/>
+  <dimension ref="A2:O15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G29" sqref="G29"/>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="J6" sqref="J6:J15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="28.5703125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.140625" customWidth="1"/>
+    <col min="7" max="7" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="28.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="16.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="N2" s="7"/>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15">
+      <c r="O2" s="7"/>
+    </row>
+    <row r="3" spans="1:15">
       <c r="A3" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="N3" s="1"/>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="N4" s="1"/>
-    </row>
-    <row r="5" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="N5" s="1"/>
-    </row>
-    <row r="6" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O3" s="1"/>
+    </row>
+    <row r="4" spans="1:15">
+      <c r="O4" s="1"/>
+    </row>
+    <row r="5" spans="1:15" ht="15.75" thickBot="1">
+      <c r="O5" s="1"/>
+    </row>
+    <row r="6" spans="1:15" ht="15.75" thickBot="1">
       <c r="B6" s="34" t="s">
         <v>8</v>
       </c>
       <c r="C6" s="35" t="s">
-        <v>26</v>
+        <v>74</v>
       </c>
       <c r="D6" s="35" t="s">
         <v>27</v>
@@ -1605,32 +2117,35 @@
         <v>0</v>
       </c>
       <c r="F6" s="35" t="s">
+        <v>73</v>
+      </c>
+      <c r="G6" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="G6" s="36" t="s">
+      <c r="H6" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="H6" s="35" t="s">
+      <c r="I6" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="I6" s="35" t="s">
+      <c r="J6" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="J6" s="35" t="s">
+      <c r="K6" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="K6" s="35" t="s">
+      <c r="L6" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="L6" s="37" t="s">
+      <c r="M6" s="37" t="s">
         <v>42</v>
       </c>
-      <c r="M6" s="38" t="s">
+      <c r="N6" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="N6" s="1"/>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O6" s="1"/>
+    </row>
+    <row r="7" spans="1:15">
       <c r="B7" s="28" t="s">
         <v>9</v>
       </c>
@@ -1641,35 +2156,38 @@
         <v>3</v>
       </c>
       <c r="E7" s="30">
-        <v>0.8</v>
+        <v>0.6</v>
       </c>
       <c r="F7" s="30">
         <v>0.2</v>
       </c>
-      <c r="G7" s="31">
+      <c r="G7" s="30">
+        <v>0.2</v>
+      </c>
+      <c r="H7" s="31">
         <v>10000</v>
       </c>
-      <c r="H7" s="30">
+      <c r="I7" s="30">
         <v>1</v>
       </c>
-      <c r="I7" s="30">
+      <c r="J7" s="30">
         <v>2500</v>
       </c>
-      <c r="J7" s="30">
+      <c r="K7" s="30">
         <v>0.1</v>
       </c>
-      <c r="K7" s="39">
+      <c r="L7" s="39">
         <v>1E-3</v>
       </c>
-      <c r="L7" s="32">
+      <c r="M7" s="32">
         <v>0.32890000000000003</v>
       </c>
-      <c r="M7" s="40" t="s">
+      <c r="N7" s="40" t="s">
         <v>40</v>
       </c>
-      <c r="N7" s="1"/>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O7" s="1"/>
+    </row>
+    <row r="8" spans="1:15">
       <c r="B8" s="12" t="s">
         <v>11</v>
       </c>
@@ -1679,36 +2197,39 @@
       <c r="D8" s="8">
         <v>3</v>
       </c>
-      <c r="E8" s="8">
-        <v>0.8</v>
-      </c>
-      <c r="F8" s="8">
-        <v>0.2</v>
-      </c>
-      <c r="G8" s="9">
+      <c r="E8" s="30">
+        <v>0.6</v>
+      </c>
+      <c r="F8" s="30">
+        <v>0.2</v>
+      </c>
+      <c r="G8" s="8">
+        <v>0.2</v>
+      </c>
+      <c r="H8" s="9">
         <v>10000</v>
       </c>
-      <c r="H8" s="8">
+      <c r="I8" s="8">
         <v>1</v>
       </c>
-      <c r="I8" s="8">
+      <c r="J8" s="8">
         <v>2500</v>
       </c>
-      <c r="J8" s="8">
+      <c r="K8" s="8">
         <v>0.1</v>
       </c>
-      <c r="K8" s="5">
+      <c r="L8" s="5">
         <v>0.1</v>
       </c>
-      <c r="L8" s="10">
+      <c r="M8" s="10">
         <v>0.54817275747508298</v>
       </c>
-      <c r="M8" s="14" t="s">
+      <c r="N8" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="N8" s="1"/>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O8" s="1"/>
+    </row>
+    <row r="9" spans="1:15">
       <c r="B9" s="12" t="s">
         <v>13</v>
       </c>
@@ -1718,36 +2239,39 @@
       <c r="D9" s="8">
         <v>3</v>
       </c>
-      <c r="E9" s="8">
-        <v>0.8</v>
-      </c>
-      <c r="F9" s="8">
-        <v>0.2</v>
-      </c>
-      <c r="G9" s="9">
+      <c r="E9" s="30">
+        <v>0.6</v>
+      </c>
+      <c r="F9" s="30">
+        <v>0.2</v>
+      </c>
+      <c r="G9" s="8">
+        <v>0.2</v>
+      </c>
+      <c r="H9" s="9">
         <v>10000</v>
       </c>
-      <c r="H9" s="8">
+      <c r="I9" s="8">
         <v>1</v>
       </c>
-      <c r="I9" s="8">
+      <c r="J9" s="8">
         <v>2500</v>
       </c>
-      <c r="J9" s="8">
+      <c r="K9" s="8">
         <v>0.1</v>
       </c>
-      <c r="K9" s="5">
+      <c r="L9" s="5">
         <v>0.01</v>
       </c>
-      <c r="L9" s="10">
+      <c r="M9" s="10">
         <v>0.54817275747508298</v>
       </c>
-      <c r="M9" s="14" t="s">
+      <c r="N9" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="N9" s="1"/>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O9" s="1"/>
+    </row>
+    <row r="10" spans="1:15">
       <c r="B10" s="12" t="s">
         <v>14</v>
       </c>
@@ -1757,36 +2281,39 @@
       <c r="D10" s="8">
         <v>3</v>
       </c>
-      <c r="E10" s="8">
-        <v>0.8</v>
-      </c>
-      <c r="F10" s="8">
-        <v>0.2</v>
-      </c>
-      <c r="G10" s="9">
+      <c r="E10" s="30">
+        <v>0.6</v>
+      </c>
+      <c r="F10" s="30">
+        <v>0.2</v>
+      </c>
+      <c r="G10" s="8">
+        <v>0.2</v>
+      </c>
+      <c r="H10" s="9">
         <v>10000</v>
       </c>
-      <c r="H10" s="8">
+      <c r="I10" s="8">
         <v>1</v>
       </c>
-      <c r="I10" s="8">
+      <c r="J10" s="8">
         <v>3500</v>
       </c>
-      <c r="J10" s="8">
+      <c r="K10" s="8">
         <v>0.1</v>
       </c>
-      <c r="K10" s="5">
+      <c r="L10" s="5">
         <v>0.03</v>
       </c>
-      <c r="L10" s="10">
+      <c r="M10" s="10">
         <v>0.59468438538205903</v>
       </c>
-      <c r="M10" s="14" t="s">
+      <c r="N10" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="N10" s="1"/>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O10" s="1"/>
+    </row>
+    <row r="11" spans="1:15">
       <c r="B11" s="12" t="s">
         <v>16</v>
       </c>
@@ -1796,36 +2323,39 @@
       <c r="D11" s="8">
         <v>3</v>
       </c>
-      <c r="E11" s="8">
-        <v>0.8</v>
-      </c>
-      <c r="F11" s="8">
-        <v>0.2</v>
-      </c>
-      <c r="G11" s="9">
+      <c r="E11" s="30">
+        <v>0.6</v>
+      </c>
+      <c r="F11" s="30">
+        <v>0.2</v>
+      </c>
+      <c r="G11" s="8">
+        <v>0.2</v>
+      </c>
+      <c r="H11" s="9">
         <v>65536</v>
       </c>
-      <c r="H11" s="8">
+      <c r="I11" s="8">
         <v>1</v>
       </c>
-      <c r="I11" s="8">
+      <c r="J11" s="8">
         <v>3500</v>
       </c>
-      <c r="J11" s="8">
+      <c r="K11" s="8">
         <v>1E-3</v>
       </c>
-      <c r="K11" s="5">
+      <c r="L11" s="5">
         <v>0.03</v>
       </c>
-      <c r="L11" s="10">
+      <c r="M11" s="10">
         <v>0.61461794019933502</v>
       </c>
-      <c r="M11" s="14" t="s">
+      <c r="N11" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="N11" s="1"/>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O11" s="1"/>
+    </row>
+    <row r="12" spans="1:15">
       <c r="B12" s="12" t="s">
         <v>19</v>
       </c>
@@ -1835,35 +2365,38 @@
       <c r="D12" s="5">
         <v>4</v>
       </c>
-      <c r="E12" s="8">
-        <v>0.8</v>
-      </c>
-      <c r="F12" s="8">
-        <v>0.2</v>
-      </c>
-      <c r="G12" s="9">
+      <c r="E12" s="30">
+        <v>0.6</v>
+      </c>
+      <c r="F12" s="30">
+        <v>0.2</v>
+      </c>
+      <c r="G12" s="8">
+        <v>0.2</v>
+      </c>
+      <c r="H12" s="9">
         <v>65536</v>
       </c>
-      <c r="H12" s="8">
+      <c r="I12" s="8">
         <v>1</v>
       </c>
-      <c r="I12" s="8">
+      <c r="J12" s="8">
         <v>3500</v>
       </c>
-      <c r="J12" s="8">
+      <c r="K12" s="8">
         <v>1E-3</v>
       </c>
-      <c r="K12" s="5">
+      <c r="L12" s="5">
         <v>0.08</v>
       </c>
-      <c r="L12" s="10">
+      <c r="M12" s="10">
         <v>0.50793650793650702</v>
       </c>
-      <c r="M12" s="14" t="s">
+      <c r="N12" s="14" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15">
       <c r="B13" s="12" t="s">
         <v>21</v>
       </c>
@@ -1873,35 +2406,38 @@
       <c r="D13" s="5">
         <v>3</v>
       </c>
-      <c r="E13" s="8">
-        <v>0.8</v>
-      </c>
-      <c r="F13" s="8">
-        <v>0.2</v>
-      </c>
-      <c r="G13" s="9">
+      <c r="E13" s="30">
+        <v>0.6</v>
+      </c>
+      <c r="F13" s="30">
+        <v>0.2</v>
+      </c>
+      <c r="G13" s="8">
+        <v>0.2</v>
+      </c>
+      <c r="H13" s="9">
         <v>65536</v>
       </c>
-      <c r="H13" s="8">
+      <c r="I13" s="8">
         <v>1</v>
       </c>
-      <c r="I13" s="5">
+      <c r="J13" s="5">
         <v>4500</v>
       </c>
-      <c r="J13" s="8">
+      <c r="K13" s="8">
         <v>1E-3</v>
       </c>
-      <c r="K13" s="5">
+      <c r="L13" s="5">
         <v>0.03</v>
       </c>
-      <c r="L13" s="10">
+      <c r="M13" s="10">
         <v>0.65116279069767402</v>
       </c>
-      <c r="M13" s="14" t="s">
+      <c r="N13" s="14" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15">
       <c r="B14" s="12" t="s">
         <v>23</v>
       </c>
@@ -1911,35 +2447,38 @@
       <c r="D14" s="5">
         <v>2</v>
       </c>
-      <c r="E14" s="8">
-        <v>0.8</v>
-      </c>
-      <c r="F14" s="8">
-        <v>0.2</v>
-      </c>
-      <c r="G14" s="9">
+      <c r="E14" s="30">
+        <v>0.6</v>
+      </c>
+      <c r="F14" s="30">
+        <v>0.2</v>
+      </c>
+      <c r="G14" s="8">
+        <v>0.2</v>
+      </c>
+      <c r="H14" s="9">
         <v>65536</v>
       </c>
-      <c r="H14" s="8">
+      <c r="I14" s="8">
         <v>1</v>
       </c>
-      <c r="I14" s="5">
+      <c r="J14" s="5">
         <v>4500</v>
       </c>
-      <c r="J14" s="8">
+      <c r="K14" s="8">
         <v>1E-3</v>
       </c>
-      <c r="K14" s="5">
+      <c r="L14" s="5">
         <v>0.03</v>
       </c>
-      <c r="L14" s="10">
+      <c r="M14" s="10">
         <v>0.45497630331753502</v>
       </c>
-      <c r="M14" s="14" t="s">
+      <c r="N14" s="14" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="15" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:15" ht="15.75" thickBot="1">
       <c r="B15" s="12" t="s">
         <v>24</v>
       </c>
@@ -1949,44 +2488,47 @@
       <c r="D15" s="17">
         <v>3</v>
       </c>
-      <c r="E15" s="16">
-        <v>0.8</v>
-      </c>
-      <c r="F15" s="16">
-        <v>0.2</v>
-      </c>
-      <c r="G15" s="18">
+      <c r="E15" s="30">
+        <v>0.6</v>
+      </c>
+      <c r="F15" s="30">
+        <v>0.2</v>
+      </c>
+      <c r="G15" s="16">
+        <v>0.2</v>
+      </c>
+      <c r="H15" s="18">
         <v>65536</v>
       </c>
-      <c r="H15" s="16">
+      <c r="I15" s="16">
         <v>1</v>
       </c>
-      <c r="I15" s="17">
+      <c r="J15" s="17">
         <v>6500</v>
       </c>
-      <c r="J15" s="16">
+      <c r="K15" s="16">
         <v>1E-3</v>
       </c>
-      <c r="K15" s="17">
+      <c r="L15" s="17">
         <v>0.03</v>
       </c>
-      <c r="L15" s="19">
+      <c r="M15" s="19">
         <v>0.62790697674418605</v>
       </c>
-      <c r="M15" s="20" t="s">
+      <c r="N15" s="20" t="s">
         <v>39</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="M8" r:id="rId1" xr:uid="{FF156B1F-80B5-4607-AA23-48A2217E6BBB}"/>
-    <hyperlink ref="M10" r:id="rId2" xr:uid="{70365747-E8F3-4AE2-9E53-71D60CCFB964}"/>
-    <hyperlink ref="M12" r:id="rId3" xr:uid="{682A0584-263C-40CF-AB0F-116C6EC36397}"/>
-    <hyperlink ref="M13" r:id="rId4" xr:uid="{83038214-89E3-4777-8E14-897175660CA2}"/>
-    <hyperlink ref="M11" r:id="rId5" xr:uid="{7EFF1BBE-EF09-4414-B8CC-0984E876294E}"/>
-    <hyperlink ref="M14" r:id="rId6" xr:uid="{07B1BDF0-D52D-4264-B9B6-ECC190B048C3}"/>
-    <hyperlink ref="M15" r:id="rId7" xr:uid="{21931E3D-FF50-471E-9E59-14E27BD44BBA}"/>
+    <hyperlink ref="N8" r:id="rId1" xr:uid="{FF156B1F-80B5-4607-AA23-48A2217E6BBB}"/>
+    <hyperlink ref="N10" r:id="rId2" xr:uid="{70365747-E8F3-4AE2-9E53-71D60CCFB964}"/>
+    <hyperlink ref="N12" r:id="rId3" xr:uid="{682A0584-263C-40CF-AB0F-116C6EC36397}"/>
+    <hyperlink ref="N13" r:id="rId4" xr:uid="{83038214-89E3-4777-8E14-897175660CA2}"/>
+    <hyperlink ref="N11" r:id="rId5" xr:uid="{7EFF1BBE-EF09-4414-B8CC-0984E876294E}"/>
+    <hyperlink ref="N14" r:id="rId6" xr:uid="{07B1BDF0-D52D-4264-B9B6-ECC190B048C3}"/>
+    <hyperlink ref="N15" r:id="rId7" xr:uid="{21931E3D-FF50-471E-9E59-14E27BD44BBA}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1996,11 +2538,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50F8050B-3B3B-492A-8F2D-EDA4E083EFA1}">
   <dimension ref="A3:O16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N16" sqref="N7:O16"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="N13" sqref="N13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.42578125" bestFit="1" customWidth="1"/>
@@ -2019,24 +2561,24 @@
     <col min="15" max="15" width="29.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15">
       <c r="A3" s="6" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="5" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="6" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:15" ht="15.75" thickBot="1"/>
+    <row r="6" spans="1:15" ht="15.75" thickBot="1">
       <c r="B6" s="29" t="s">
-        <v>8</v>
+        <v>76</v>
       </c>
       <c r="C6" s="45" t="s">
-        <v>26</v>
+        <v>75</v>
       </c>
       <c r="D6" s="35" t="s">
-        <v>27</v>
+        <v>77</v>
       </c>
       <c r="E6" s="35" t="s">
-        <v>0</v>
+        <v>78</v>
       </c>
       <c r="F6" s="35" t="s">
         <v>1</v>
@@ -2048,7 +2590,7 @@
         <v>3</v>
       </c>
       <c r="I6" s="46" t="s">
-        <v>4</v>
+        <v>79</v>
       </c>
       <c r="J6" s="35" t="s">
         <v>5</v>
@@ -2057,10 +2599,10 @@
         <v>6</v>
       </c>
       <c r="L6" s="37" t="s">
-        <v>43</v>
+        <v>80</v>
       </c>
       <c r="M6" s="47" t="s">
-        <v>42</v>
+        <v>81</v>
       </c>
       <c r="N6" s="47" t="s">
         <v>45</v>
@@ -2069,7 +2611,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15">
       <c r="B7" s="23" t="s">
         <v>9</v>
       </c>
@@ -2113,7 +2655,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15">
       <c r="B8" s="12" t="s">
         <v>11</v>
       </c>
@@ -2157,7 +2699,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15">
       <c r="B9" s="12" t="s">
         <v>13</v>
       </c>
@@ -2201,7 +2743,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15">
       <c r="B10" s="12" t="s">
         <v>14</v>
       </c>
@@ -2245,7 +2787,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15">
       <c r="B11" s="12" t="s">
         <v>16</v>
       </c>
@@ -2289,7 +2831,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15">
       <c r="B12" s="12" t="s">
         <v>19</v>
       </c>
@@ -2333,7 +2875,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15">
       <c r="B13" s="12" t="s">
         <v>21</v>
       </c>
@@ -2377,7 +2919,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15">
       <c r="B14" s="12" t="s">
         <v>23</v>
       </c>
@@ -2421,7 +2963,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15">
       <c r="B15" s="12" t="s">
         <v>24</v>
       </c>
@@ -2465,7 +3007,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="16" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:15" ht="15.75" thickBot="1">
       <c r="B16" s="48" t="s">
         <v>31</v>
       </c>
@@ -2536,4 +3078,967 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId21"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3866BA57-CFCF-4B34-94F4-765385899DE4}">
+  <dimension ref="A3:O18"/>
+  <sheetViews>
+    <sheetView topLeftCell="G4" workbookViewId="0">
+      <selection activeCell="N12" sqref="N12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="29.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:15">
+      <c r="A3" s="6" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" ht="15.75" thickBot="1"/>
+    <row r="6" spans="1:15" ht="15.75" thickBot="1">
+      <c r="B6" s="29" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="45" t="s">
+        <v>26</v>
+      </c>
+      <c r="D6" s="35" t="s">
+        <v>27</v>
+      </c>
+      <c r="E6" s="35" t="s">
+        <v>0</v>
+      </c>
+      <c r="F6" s="35" t="s">
+        <v>1</v>
+      </c>
+      <c r="G6" s="36" t="s">
+        <v>2</v>
+      </c>
+      <c r="H6" s="35" t="s">
+        <v>3</v>
+      </c>
+      <c r="I6" s="46" t="s">
+        <v>4</v>
+      </c>
+      <c r="J6" s="35" t="s">
+        <v>5</v>
+      </c>
+      <c r="K6" s="45" t="s">
+        <v>6</v>
+      </c>
+      <c r="L6" s="37" t="s">
+        <v>43</v>
+      </c>
+      <c r="M6" s="47" t="s">
+        <v>42</v>
+      </c>
+      <c r="N6" s="47" t="s">
+        <v>45</v>
+      </c>
+      <c r="O6" s="38" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15">
+      <c r="B7" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="24" t="s">
+        <v>29</v>
+      </c>
+      <c r="D7" s="11">
+        <v>3</v>
+      </c>
+      <c r="E7" s="24">
+        <v>0.8</v>
+      </c>
+      <c r="F7" s="24">
+        <v>0.2</v>
+      </c>
+      <c r="G7" s="25">
+        <v>10000</v>
+      </c>
+      <c r="H7" s="24">
+        <v>9</v>
+      </c>
+      <c r="I7" s="43">
+        <v>5000</v>
+      </c>
+      <c r="J7" s="24">
+        <v>1E-3</v>
+      </c>
+      <c r="K7" s="44">
+        <v>0.03</v>
+      </c>
+      <c r="L7" s="42">
+        <v>0.84608985024958405</v>
+      </c>
+      <c r="M7" s="42">
+        <v>0.72093023255813904</v>
+      </c>
+      <c r="N7" s="26" t="s">
+        <v>71</v>
+      </c>
+      <c r="O7" s="27" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15">
+      <c r="B8" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="D8" s="5">
+        <v>3</v>
+      </c>
+      <c r="E8" s="8">
+        <v>0.8</v>
+      </c>
+      <c r="F8" s="8">
+        <v>0.2</v>
+      </c>
+      <c r="G8" s="9">
+        <v>10000</v>
+      </c>
+      <c r="H8" s="8">
+        <v>9</v>
+      </c>
+      <c r="I8" s="2">
+        <v>10000</v>
+      </c>
+      <c r="J8" s="30">
+        <v>1E-3</v>
+      </c>
+      <c r="K8" s="72">
+        <v>0.03</v>
+      </c>
+      <c r="L8" s="54"/>
+      <c r="M8" s="54"/>
+      <c r="N8" s="21"/>
+      <c r="O8" s="41"/>
+    </row>
+    <row r="9" spans="1:15">
+      <c r="B9" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="D9" s="5">
+        <v>3</v>
+      </c>
+      <c r="E9" s="8">
+        <v>0.8</v>
+      </c>
+      <c r="F9" s="8">
+        <v>0.2</v>
+      </c>
+      <c r="G9" s="9">
+        <v>10000</v>
+      </c>
+      <c r="H9" s="8">
+        <v>9</v>
+      </c>
+      <c r="I9" s="2">
+        <v>5000</v>
+      </c>
+      <c r="J9" s="22">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="K9" s="22">
+        <v>0.01</v>
+      </c>
+      <c r="L9" s="54">
+        <v>0.80698835274542402</v>
+      </c>
+      <c r="M9" s="54">
+        <v>0.73089700996677698</v>
+      </c>
+      <c r="N9" s="21" t="s">
+        <v>84</v>
+      </c>
+      <c r="O9" s="41" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15">
+      <c r="B10" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="D10" s="5">
+        <v>3</v>
+      </c>
+      <c r="E10" s="8">
+        <v>0.8</v>
+      </c>
+      <c r="F10" s="8">
+        <v>0.2</v>
+      </c>
+      <c r="G10" s="9">
+        <v>10000</v>
+      </c>
+      <c r="H10" s="8">
+        <v>9</v>
+      </c>
+      <c r="I10" s="2">
+        <v>10000</v>
+      </c>
+      <c r="J10" s="30">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="K10" s="72">
+        <v>0.01</v>
+      </c>
+      <c r="L10" s="54"/>
+      <c r="M10" s="54"/>
+      <c r="N10" s="21"/>
+      <c r="O10" s="41"/>
+    </row>
+    <row r="11" spans="1:15">
+      <c r="B11" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="D11" s="5">
+        <v>3</v>
+      </c>
+      <c r="E11" s="8">
+        <v>0.8</v>
+      </c>
+      <c r="F11" s="8">
+        <v>0.2</v>
+      </c>
+      <c r="G11" s="9">
+        <v>10000</v>
+      </c>
+      <c r="H11" s="22">
+        <v>15</v>
+      </c>
+      <c r="I11" s="71">
+        <v>5000</v>
+      </c>
+      <c r="J11" s="30">
+        <v>1E-3</v>
+      </c>
+      <c r="K11" s="72">
+        <v>0.03</v>
+      </c>
+      <c r="L11" s="54">
+        <v>0.80449251247920095</v>
+      </c>
+      <c r="M11" s="54">
+        <v>0.73421926910298996</v>
+      </c>
+      <c r="N11" s="21" t="s">
+        <v>82</v>
+      </c>
+      <c r="O11" s="41" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15">
+      <c r="B12" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="D12" s="5">
+        <v>3</v>
+      </c>
+      <c r="E12" s="8">
+        <v>0.8</v>
+      </c>
+      <c r="F12" s="8">
+        <v>0.2</v>
+      </c>
+      <c r="G12" s="9">
+        <v>10000</v>
+      </c>
+      <c r="H12" s="22">
+        <v>15</v>
+      </c>
+      <c r="I12" s="2">
+        <v>10000</v>
+      </c>
+      <c r="J12" s="30">
+        <v>1E-3</v>
+      </c>
+      <c r="K12" s="72">
+        <v>0.03</v>
+      </c>
+      <c r="L12" s="54">
+        <v>0.86439267886855198</v>
+      </c>
+      <c r="M12" s="54">
+        <v>0.76744186046511598</v>
+      </c>
+      <c r="N12" s="21" t="s">
+        <v>86</v>
+      </c>
+      <c r="O12" s="41" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15">
+      <c r="B13" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="D13" s="5">
+        <v>3</v>
+      </c>
+      <c r="E13" s="8">
+        <v>0.8</v>
+      </c>
+      <c r="F13" s="8">
+        <v>0.2</v>
+      </c>
+      <c r="G13" s="9">
+        <v>10000</v>
+      </c>
+      <c r="H13" s="22">
+        <v>15</v>
+      </c>
+      <c r="I13" s="2">
+        <v>5000</v>
+      </c>
+      <c r="J13" s="22">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="K13" s="22">
+        <v>0.01</v>
+      </c>
+      <c r="L13" s="55"/>
+      <c r="M13" s="58"/>
+      <c r="N13" s="21"/>
+      <c r="O13" s="41"/>
+    </row>
+    <row r="14" spans="1:15">
+      <c r="B14" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="D14" s="5">
+        <v>3</v>
+      </c>
+      <c r="E14" s="8">
+        <v>0.8</v>
+      </c>
+      <c r="F14" s="8">
+        <v>0.2</v>
+      </c>
+      <c r="G14" s="9">
+        <v>10000</v>
+      </c>
+      <c r="H14" s="22">
+        <v>15</v>
+      </c>
+      <c r="I14" s="2">
+        <v>10000</v>
+      </c>
+      <c r="J14" s="30">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="K14" s="72">
+        <v>0.01</v>
+      </c>
+      <c r="L14" s="54">
+        <v>0.88269550748752001</v>
+      </c>
+      <c r="M14" s="54">
+        <v>0.78737541528239197</v>
+      </c>
+      <c r="N14" s="21" t="s">
+        <v>105</v>
+      </c>
+      <c r="O14" s="41" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15">
+      <c r="B15" s="66" t="s">
+        <v>24</v>
+      </c>
+      <c r="C15" s="67" t="s">
+        <v>29</v>
+      </c>
+      <c r="D15" s="5">
+        <v>3</v>
+      </c>
+      <c r="E15" s="8">
+        <v>0.8</v>
+      </c>
+      <c r="F15" s="8">
+        <v>0.2</v>
+      </c>
+      <c r="G15" s="9">
+        <v>10000</v>
+      </c>
+      <c r="H15" s="22">
+        <v>20</v>
+      </c>
+      <c r="I15" s="5">
+        <v>10000</v>
+      </c>
+      <c r="J15" s="8">
+        <v>0.01</v>
+      </c>
+      <c r="K15" s="5">
+        <v>0.01</v>
+      </c>
+      <c r="L15" s="55">
+        <v>0.86439267886855198</v>
+      </c>
+      <c r="M15" s="55">
+        <v>0.76744186046511598</v>
+      </c>
+      <c r="N15" s="53" t="s">
+        <v>111</v>
+      </c>
+      <c r="O15" s="14" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15">
+      <c r="B16" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="C16" s="65" t="s">
+        <v>29</v>
+      </c>
+      <c r="D16" s="5">
+        <v>3</v>
+      </c>
+      <c r="E16" s="8">
+        <v>0.8</v>
+      </c>
+      <c r="F16" s="8">
+        <v>0.2</v>
+      </c>
+      <c r="G16" s="9">
+        <v>10000</v>
+      </c>
+      <c r="H16" s="22">
+        <v>20</v>
+      </c>
+      <c r="I16" s="5"/>
+      <c r="J16" s="22"/>
+      <c r="K16" s="22"/>
+      <c r="L16" s="62"/>
+      <c r="M16" s="63"/>
+      <c r="N16" s="21"/>
+      <c r="O16" s="21"/>
+    </row>
+    <row r="17" spans="2:15">
+      <c r="B17" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="C17" s="65" t="s">
+        <v>68</v>
+      </c>
+      <c r="D17" s="5">
+        <v>3</v>
+      </c>
+      <c r="E17" s="8">
+        <v>0.8</v>
+      </c>
+      <c r="F17" s="8">
+        <v>0.2</v>
+      </c>
+      <c r="G17" s="9">
+        <v>10000</v>
+      </c>
+      <c r="H17" s="22">
+        <v>20</v>
+      </c>
+      <c r="I17" s="5"/>
+      <c r="J17" s="8"/>
+      <c r="K17" s="5"/>
+      <c r="L17" s="55"/>
+      <c r="M17" s="55"/>
+      <c r="N17" s="53"/>
+      <c r="O17" s="64"/>
+    </row>
+    <row r="18" spans="2:15" ht="15.75" thickBot="1">
+      <c r="B18" s="48" t="s">
+        <v>69</v>
+      </c>
+      <c r="C18" s="49" t="s">
+        <v>70</v>
+      </c>
+      <c r="D18" s="50">
+        <v>3</v>
+      </c>
+      <c r="E18" s="49">
+        <v>0.8</v>
+      </c>
+      <c r="F18" s="49">
+        <v>0.2</v>
+      </c>
+      <c r="G18" s="68">
+        <v>10000</v>
+      </c>
+      <c r="H18" s="70">
+        <v>20</v>
+      </c>
+      <c r="I18" s="69"/>
+      <c r="J18" s="59"/>
+      <c r="K18" s="59"/>
+      <c r="L18" s="56"/>
+      <c r="M18" s="57"/>
+      <c r="N18" s="60"/>
+      <c r="O18" s="61"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="5" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="N7" r:id="rId1" xr:uid="{D22DED53-231D-4FA7-BCB0-A25A89B5065F}"/>
+    <hyperlink ref="O7" r:id="rId2" xr:uid="{D864631C-3D57-4DB6-9D0E-41A56306F3FD}"/>
+    <hyperlink ref="N11" r:id="rId3" xr:uid="{3A243E82-1CB3-4D42-BD3A-33E52FF157E9}"/>
+    <hyperlink ref="O11" r:id="rId4" xr:uid="{DC027FAF-49D5-4EDF-941C-0532991EA697}"/>
+    <hyperlink ref="N9" r:id="rId5" xr:uid="{B6BE1945-F487-4886-BE4B-1F88956EF503}"/>
+    <hyperlink ref="O9" r:id="rId6" xr:uid="{9FB1C9B4-2C27-4FEB-BDDB-1A26434135B6}"/>
+    <hyperlink ref="N12" r:id="rId7" xr:uid="{F937DDF1-C004-4425-ACF7-87525BBC38F1}"/>
+    <hyperlink ref="O12" r:id="rId8" xr:uid="{2444CF7E-A702-4877-8911-CCD94F78E210}"/>
+    <hyperlink ref="N14" r:id="rId9" xr:uid="{B4CB9A64-5A41-4B25-9DA4-2A64C4DA1840}"/>
+    <hyperlink ref="O14" r:id="rId10" xr:uid="{1A041FEA-7C3B-414D-9356-E9A3B80D88A7}"/>
+    <hyperlink ref="O15" r:id="rId11" xr:uid="{B57CC596-4568-460F-AD5B-C757DE7D99F5}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F52DCBD4-48A4-41FB-95FF-357BE45DA84F}">
+  <dimension ref="B4:N17"/>
+  <sheetViews>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="N9" sqref="N9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="3" max="3" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.28515625" customWidth="1"/>
+    <col min="12" max="12" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.7109375" customWidth="1"/>
+    <col min="14" max="14" width="15.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="2:14" ht="15.75" thickBot="1"/>
+    <row r="5" spans="2:14" ht="15.75" thickBot="1">
+      <c r="K5" s="92" t="s">
+        <v>92</v>
+      </c>
+      <c r="L5" s="93"/>
+      <c r="M5" s="93"/>
+      <c r="N5" s="94"/>
+    </row>
+    <row r="6" spans="2:14" ht="15.75" thickBot="1">
+      <c r="B6" s="80" t="s">
+        <v>76</v>
+      </c>
+      <c r="C6" s="81" t="s">
+        <v>75</v>
+      </c>
+      <c r="D6" s="82" t="s">
+        <v>77</v>
+      </c>
+      <c r="E6" s="82" t="s">
+        <v>78</v>
+      </c>
+      <c r="F6" s="82" t="s">
+        <v>1</v>
+      </c>
+      <c r="G6" s="82" t="s">
+        <v>100</v>
+      </c>
+      <c r="H6" s="82" t="s">
+        <v>4</v>
+      </c>
+      <c r="I6" s="83" t="s">
+        <v>43</v>
+      </c>
+      <c r="J6" s="84" t="s">
+        <v>42</v>
+      </c>
+      <c r="K6" s="91" t="s">
+        <v>91</v>
+      </c>
+      <c r="L6" s="88" t="s">
+        <v>88</v>
+      </c>
+      <c r="M6" s="88" t="s">
+        <v>89</v>
+      </c>
+      <c r="N6" s="89" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="7" spans="2:14">
+      <c r="B7" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="24" t="s">
+        <v>29</v>
+      </c>
+      <c r="D7" s="11">
+        <v>3</v>
+      </c>
+      <c r="E7" s="24">
+        <v>0.8</v>
+      </c>
+      <c r="F7" s="24">
+        <v>0.2</v>
+      </c>
+      <c r="G7" s="24" t="s">
+        <v>101</v>
+      </c>
+      <c r="H7" s="24">
+        <v>20000</v>
+      </c>
+      <c r="I7" s="42">
+        <v>0.99750415973377704</v>
+      </c>
+      <c r="J7" s="78">
+        <v>0.77076411960132896</v>
+      </c>
+      <c r="K7" s="95" t="s">
+        <v>90</v>
+      </c>
+      <c r="L7" s="87" t="s">
+        <v>93</v>
+      </c>
+      <c r="M7" s="87" t="s">
+        <v>117</v>
+      </c>
+      <c r="N7" s="85" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="8" spans="2:14">
+      <c r="B8" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="D8" s="5">
+        <v>3</v>
+      </c>
+      <c r="E8" s="8">
+        <v>0.7</v>
+      </c>
+      <c r="F8" s="8">
+        <v>0.3</v>
+      </c>
+      <c r="G8" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="H8" s="8">
+        <v>20000</v>
+      </c>
+      <c r="I8" s="54">
+        <v>0.99904942965779397</v>
+      </c>
+      <c r="J8" s="79">
+        <v>0.77827050997782699</v>
+      </c>
+      <c r="K8" s="74" t="s">
+        <v>99</v>
+      </c>
+      <c r="L8" s="74" t="s">
+        <v>98</v>
+      </c>
+      <c r="M8" s="74" t="s">
+        <v>97</v>
+      </c>
+      <c r="N8" s="75" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="9" spans="2:14" ht="15.75" thickBot="1">
+      <c r="B9" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="D9" s="17">
+        <v>3</v>
+      </c>
+      <c r="E9" s="16">
+        <v>0.6</v>
+      </c>
+      <c r="F9" s="16">
+        <v>0.2</v>
+      </c>
+      <c r="G9" s="16">
+        <v>0.2</v>
+      </c>
+      <c r="H9" s="16">
+        <v>20000</v>
+      </c>
+      <c r="I9" s="76">
+        <v>1</v>
+      </c>
+      <c r="J9" s="98">
+        <v>0.79734219269103002</v>
+      </c>
+      <c r="K9" s="86" t="s">
+        <v>104</v>
+      </c>
+      <c r="L9" s="86" t="s">
+        <v>118</v>
+      </c>
+      <c r="M9" s="99" t="s">
+        <v>103</v>
+      </c>
+      <c r="N9" s="77" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="10" spans="2:14" ht="15.75" thickBot="1">
+      <c r="B10" s="96"/>
+      <c r="C10" s="97"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="97"/>
+      <c r="F10" s="97"/>
+      <c r="G10" s="97"/>
+      <c r="H10" s="97"/>
+      <c r="I10" s="73"/>
+      <c r="J10" s="73"/>
+      <c r="K10" s="90"/>
+      <c r="L10" s="90"/>
+      <c r="M10" s="90"/>
+      <c r="N10" s="90"/>
+    </row>
+    <row r="11" spans="2:14" ht="15.75" thickBot="1">
+      <c r="K11" s="92" t="s">
+        <v>92</v>
+      </c>
+      <c r="L11" s="93"/>
+      <c r="M11" s="93"/>
+      <c r="N11" s="94"/>
+    </row>
+    <row r="12" spans="2:14" ht="15.75" thickBot="1">
+      <c r="B12" s="80" t="s">
+        <v>76</v>
+      </c>
+      <c r="C12" s="81" t="s">
+        <v>75</v>
+      </c>
+      <c r="D12" s="82" t="s">
+        <v>77</v>
+      </c>
+      <c r="E12" s="82" t="s">
+        <v>78</v>
+      </c>
+      <c r="F12" s="82" t="s">
+        <v>1</v>
+      </c>
+      <c r="G12" s="82" t="s">
+        <v>100</v>
+      </c>
+      <c r="H12" s="82" t="s">
+        <v>4</v>
+      </c>
+      <c r="I12" s="83" t="s">
+        <v>43</v>
+      </c>
+      <c r="J12" s="84" t="s">
+        <v>42</v>
+      </c>
+      <c r="K12" s="91" t="s">
+        <v>91</v>
+      </c>
+      <c r="L12" s="88" t="s">
+        <v>88</v>
+      </c>
+      <c r="M12" s="88" t="s">
+        <v>89</v>
+      </c>
+      <c r="N12" s="89" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="13" spans="2:14" ht="15.75" thickBot="1">
+      <c r="B13" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" s="24" t="s">
+        <v>29</v>
+      </c>
+      <c r="D13" s="11">
+        <v>3</v>
+      </c>
+      <c r="E13" s="24">
+        <v>0.8</v>
+      </c>
+      <c r="F13" s="24">
+        <v>0.2</v>
+      </c>
+      <c r="G13" s="24" t="s">
+        <v>101</v>
+      </c>
+      <c r="H13" s="24">
+        <v>20000</v>
+      </c>
+      <c r="I13" s="76">
+        <v>1</v>
+      </c>
+      <c r="J13" s="100">
+        <v>0.76744186046511598</v>
+      </c>
+      <c r="K13" s="95" t="s">
+        <v>115</v>
+      </c>
+      <c r="L13" s="87" t="s">
+        <v>114</v>
+      </c>
+      <c r="M13" s="87" t="s">
+        <v>113</v>
+      </c>
+      <c r="N13" s="85" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="14" spans="2:14" ht="15.75" thickBot="1">
+      <c r="B14" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="D14" s="5">
+        <v>3</v>
+      </c>
+      <c r="E14" s="8">
+        <v>0.7</v>
+      </c>
+      <c r="F14" s="8">
+        <v>0.3</v>
+      </c>
+      <c r="G14" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="H14" s="8">
+        <v>20000</v>
+      </c>
+      <c r="I14" s="76">
+        <v>1</v>
+      </c>
+      <c r="J14" s="79">
+        <v>0.76940133037694003</v>
+      </c>
+      <c r="K14" s="74" t="s">
+        <v>99</v>
+      </c>
+      <c r="L14" s="74" t="s">
+        <v>98</v>
+      </c>
+      <c r="M14" s="74" t="s">
+        <v>97</v>
+      </c>
+      <c r="N14" s="75" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="15" spans="2:14" ht="15.75" thickBot="1">
+      <c r="B15" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="C15" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="D15" s="17">
+        <v>3</v>
+      </c>
+      <c r="E15" s="16">
+        <v>0.6</v>
+      </c>
+      <c r="F15" s="16">
+        <v>0.2</v>
+      </c>
+      <c r="G15" s="16">
+        <v>0.2</v>
+      </c>
+      <c r="H15" s="16">
+        <v>20000</v>
+      </c>
+      <c r="I15" s="76">
+        <v>1</v>
+      </c>
+      <c r="J15" s="98">
+        <v>0.77408637873754105</v>
+      </c>
+      <c r="K15" s="86" t="s">
+        <v>107</v>
+      </c>
+      <c r="L15" s="86" t="s">
+        <v>108</v>
+      </c>
+      <c r="M15" s="99" t="s">
+        <v>109</v>
+      </c>
+      <c r="N15" s="77" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="16" spans="2:14">
+      <c r="B16" s="96"/>
+      <c r="C16" s="97"/>
+      <c r="D16" s="7"/>
+      <c r="E16" s="97"/>
+      <c r="F16" s="97"/>
+      <c r="G16" s="97"/>
+      <c r="H16" s="97"/>
+      <c r="I16" s="73"/>
+      <c r="J16" s="90"/>
+      <c r="K16" s="90"/>
+      <c r="L16" s="90"/>
+      <c r="M16" s="90"/>
+      <c r="N16" s="90"/>
+    </row>
+    <row r="17" spans="9:9">
+      <c r="I17" s="73"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="K5:N5"/>
+    <mergeCell ref="K11:N11"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Adds report and presentation and final excel for tests
</commit_message>
<xml_diff>
--- a/TestsForNN.xlsx
+++ b/TestsForNN.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\biaco\MEOCloud\UA\AA\Projeto\AA-Projeto1-main\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E338E283-EC30-4CBB-98B1-7B597A3A9134}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1F81829-B3A6-4820-BA9F-4F4627396627}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9195" yWindow="2460" windowWidth="18495" windowHeight="11385" activeTab="2" xr2:uid="{4F881D6F-E29F-4FDB-B849-47811DDC3998}"/>
+    <workbookView xWindow="40860" yWindow="-195" windowWidth="14655" windowHeight="11385" activeTab="3" xr2:uid="{4F881D6F-E29F-4FDB-B849-47811DDC3998}"/>
   </bookViews>
   <sheets>
     <sheet name="1st Phase" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="119">
   <si>
     <t>Training Set</t>
   </si>
@@ -242,18 +242,6 @@
     <t>4th Phase</t>
   </si>
   <si>
-    <t>#11</t>
-  </si>
-  <si>
-    <t>100x101</t>
-  </si>
-  <si>
-    <t>#12</t>
-  </si>
-  <si>
-    <t>100x102</t>
-  </si>
-  <si>
     <t>https://imgur.com/a/Lkcypmi</t>
   </si>
   <si>
@@ -396,6 +384,18 @@
   </si>
   <si>
     <t>71.667%/ 71.111%</t>
+  </si>
+  <si>
+    <t>https://imgur.com/a/loqceWv</t>
+  </si>
+  <si>
+    <t>https://imgur.com/a/wDtOqA1</t>
+  </si>
+  <si>
+    <t>https://imgur.com/a/lM2LA8g</t>
+  </si>
+  <si>
+    <t>https://imgur.com/a/E8QUduv</t>
   </si>
 </sst>
 </file>
@@ -471,7 +471,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="44">
+  <borders count="41">
     <border>
       <left/>
       <right/>
@@ -818,7 +818,7 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
+      <left style="thin">
         <color indexed="64"/>
       </left>
       <right style="thin">
@@ -828,41 +828,6 @@
         <color indexed="64"/>
       </top>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -1046,7 +1011,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="101">
+  <cellXfs count="96">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1231,37 +1196,19 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="25" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1276,45 +1223,36 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1325,14 +1263,26 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="10" fontId="6" fillId="0" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="10" fontId="6" fillId="0" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1653,7 +1603,7 @@
   <dimension ref="A2:N22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6:L14"/>
+      <selection activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2066,8 +2016,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{632B25C1-EED0-43FB-9A19-E2017DDCB1BC}">
   <dimension ref="A2:O15"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6:J15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N10" sqref="N10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2108,7 +2058,7 @@
         <v>8</v>
       </c>
       <c r="C6" s="35" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D6" s="35" t="s">
         <v>27</v>
@@ -2117,7 +2067,7 @@
         <v>0</v>
       </c>
       <c r="F6" s="35" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="G6" s="35" t="s">
         <v>1</v>
@@ -2538,8 +2488,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50F8050B-3B3B-492A-8F2D-EDA4E083EFA1}">
   <dimension ref="A3:O16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="N13" sqref="N13"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2569,16 +2519,16 @@
     <row r="5" spans="1:15" ht="15.75" thickBot="1"/>
     <row r="6" spans="1:15" ht="15.75" thickBot="1">
       <c r="B6" s="29" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="C6" s="45" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="D6" s="35" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="E6" s="35" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="F6" s="35" t="s">
         <v>1</v>
@@ -2590,7 +2540,7 @@
         <v>3</v>
       </c>
       <c r="I6" s="46" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="J6" s="35" t="s">
         <v>5</v>
@@ -2599,10 +2549,10 @@
         <v>6</v>
       </c>
       <c r="L6" s="37" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="M6" s="47" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="N6" s="47" t="s">
         <v>45</v>
@@ -3082,10 +3032,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3866BA57-CFCF-4B34-94F4-765385899DE4}">
-  <dimension ref="A3:O18"/>
+  <dimension ref="A3:O15"/>
   <sheetViews>
-    <sheetView topLeftCell="G4" workbookViewId="0">
-      <selection activeCell="N12" sqref="N12"/>
+    <sheetView tabSelected="1" topLeftCell="I4" workbookViewId="0">
+      <selection activeCell="L14" sqref="L14:M14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3155,7 +3105,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:15">
+    <row r="7" spans="1:15" ht="15.75" thickBot="1">
       <c r="B7" s="23" t="s">
         <v>9</v>
       </c>
@@ -3193,14 +3143,14 @@
         <v>0.72093023255813904</v>
       </c>
       <c r="N7" s="26" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="O7" s="27" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15">
-      <c r="B8" s="12" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" ht="15.75" thickBot="1">
+      <c r="B8" s="23" t="s">
         <v>11</v>
       </c>
       <c r="C8" s="8" t="s">
@@ -3222,21 +3172,29 @@
         <v>9</v>
       </c>
       <c r="I8" s="2">
-        <v>10000</v>
-      </c>
-      <c r="J8" s="30">
-        <v>1E-3</v>
-      </c>
-      <c r="K8" s="72">
-        <v>0.03</v>
-      </c>
-      <c r="L8" s="54"/>
-      <c r="M8" s="54"/>
-      <c r="N8" s="21"/>
-      <c r="O8" s="41"/>
-    </row>
-    <row r="9" spans="1:15">
-      <c r="B9" s="12" t="s">
+        <v>5000</v>
+      </c>
+      <c r="J8" s="22">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="K8" s="22">
+        <v>0.01</v>
+      </c>
+      <c r="L8" s="54">
+        <v>0.80698835274542402</v>
+      </c>
+      <c r="M8" s="54">
+        <v>0.73089700996677698</v>
+      </c>
+      <c r="N8" s="21" t="s">
+        <v>80</v>
+      </c>
+      <c r="O8" s="41" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" ht="15.75" thickBot="1">
+      <c r="B9" s="23" t="s">
         <v>13</v>
       </c>
       <c r="C9" s="8" t="s">
@@ -3254,33 +3212,33 @@
       <c r="G9" s="9">
         <v>10000</v>
       </c>
-      <c r="H9" s="8">
-        <v>9</v>
-      </c>
-      <c r="I9" s="2">
+      <c r="H9" s="22">
+        <v>15</v>
+      </c>
+      <c r="I9" s="65">
         <v>5000</v>
       </c>
-      <c r="J9" s="22">
-        <v>3.0000000000000001E-3</v>
-      </c>
-      <c r="K9" s="22">
-        <v>0.01</v>
+      <c r="J9" s="30">
+        <v>1E-3</v>
+      </c>
+      <c r="K9" s="66">
+        <v>0.03</v>
       </c>
       <c r="L9" s="54">
-        <v>0.80698835274542402</v>
+        <v>0.80449251247920095</v>
       </c>
       <c r="M9" s="54">
-        <v>0.73089700996677698</v>
+        <v>0.73421926910298996</v>
       </c>
       <c r="N9" s="21" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="O9" s="41" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15">
-      <c r="B10" s="12" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" ht="15.75" thickBot="1">
+      <c r="B10" s="23" t="s">
         <v>14</v>
       </c>
       <c r="C10" s="8" t="s">
@@ -3298,25 +3256,33 @@
       <c r="G10" s="9">
         <v>10000</v>
       </c>
-      <c r="H10" s="8">
-        <v>9</v>
+      <c r="H10" s="22">
+        <v>15</v>
       </c>
       <c r="I10" s="2">
         <v>10000</v>
       </c>
       <c r="J10" s="30">
-        <v>3.0000000000000001E-3</v>
-      </c>
-      <c r="K10" s="72">
-        <v>0.01</v>
-      </c>
-      <c r="L10" s="54"/>
-      <c r="M10" s="54"/>
-      <c r="N10" s="21"/>
-      <c r="O10" s="41"/>
-    </row>
-    <row r="11" spans="1:15">
-      <c r="B11" s="12" t="s">
+        <v>1E-3</v>
+      </c>
+      <c r="K10" s="66">
+        <v>0.03</v>
+      </c>
+      <c r="L10" s="54">
+        <v>0.86439267886855198</v>
+      </c>
+      <c r="M10" s="54">
+        <v>0.76744186046511598</v>
+      </c>
+      <c r="N10" s="21" t="s">
+        <v>82</v>
+      </c>
+      <c r="O10" s="41" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" ht="15.75" thickBot="1">
+      <c r="B11" s="23" t="s">
         <v>16</v>
       </c>
       <c r="C11" s="8" t="s">
@@ -3337,33 +3303,33 @@
       <c r="H11" s="22">
         <v>15</v>
       </c>
-      <c r="I11" s="71">
-        <v>5000</v>
+      <c r="I11" s="2">
+        <v>10000</v>
       </c>
       <c r="J11" s="30">
-        <v>1E-3</v>
-      </c>
-      <c r="K11" s="72">
-        <v>0.03</v>
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="K11" s="66">
+        <v>0.01</v>
       </c>
       <c r="L11" s="54">
-        <v>0.80449251247920095</v>
+        <v>0.88269550748752001</v>
       </c>
       <c r="M11" s="54">
-        <v>0.73421926910298996</v>
+        <v>0.78737541528239197</v>
       </c>
       <c r="N11" s="21" t="s">
-        <v>82</v>
+        <v>101</v>
       </c>
       <c r="O11" s="41" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15">
-      <c r="B12" s="12" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" ht="15.75" thickBot="1">
+      <c r="B12" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="C12" s="8" t="s">
+      <c r="C12" s="64" t="s">
         <v>29</v>
       </c>
       <c r="D12" s="5">
@@ -3379,35 +3345,35 @@
         <v>10000</v>
       </c>
       <c r="H12" s="22">
-        <v>15</v>
-      </c>
-      <c r="I12" s="2">
+        <v>20</v>
+      </c>
+      <c r="I12" s="5">
         <v>10000</v>
       </c>
-      <c r="J12" s="30">
-        <v>1E-3</v>
-      </c>
-      <c r="K12" s="72">
-        <v>0.03</v>
-      </c>
-      <c r="L12" s="54">
+      <c r="J12" s="8">
+        <v>0.01</v>
+      </c>
+      <c r="K12" s="5">
+        <v>0.01</v>
+      </c>
+      <c r="L12" s="55">
         <v>0.86439267886855198</v>
       </c>
-      <c r="M12" s="54">
+      <c r="M12" s="55">
         <v>0.76744186046511598</v>
       </c>
-      <c r="N12" s="21" t="s">
-        <v>86</v>
-      </c>
-      <c r="O12" s="41" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15">
-      <c r="B13" s="12" t="s">
+      <c r="N12" s="53" t="s">
+        <v>107</v>
+      </c>
+      <c r="O12" s="14" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" ht="15.75" thickBot="1">
+      <c r="B13" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="C13" s="8" t="s">
+      <c r="C13" s="63" t="s">
         <v>29</v>
       </c>
       <c r="D13" s="5">
@@ -3423,10 +3389,10 @@
         <v>10000</v>
       </c>
       <c r="H13" s="22">
-        <v>15</v>
-      </c>
-      <c r="I13" s="2">
-        <v>5000</v>
+        <v>20</v>
+      </c>
+      <c r="I13" s="5">
+        <v>15000</v>
       </c>
       <c r="J13" s="22">
         <v>3.0000000000000001E-3</v>
@@ -3434,16 +3400,24 @@
       <c r="K13" s="22">
         <v>0.01</v>
       </c>
-      <c r="L13" s="55"/>
-      <c r="M13" s="58"/>
-      <c r="N13" s="21"/>
-      <c r="O13" s="41"/>
+      <c r="L13" s="91">
+        <v>0.95590682196339405</v>
+      </c>
+      <c r="M13" s="55">
+        <v>0.78405315614617899</v>
+      </c>
+      <c r="N13" s="21" t="s">
+        <v>115</v>
+      </c>
+      <c r="O13" s="21" t="s">
+        <v>116</v>
+      </c>
     </row>
     <row r="14" spans="1:15">
-      <c r="B14" s="12" t="s">
+      <c r="B14" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="C14" s="8" t="s">
+      <c r="C14" s="63" t="s">
         <v>29</v>
       </c>
       <c r="D14" s="5">
@@ -3459,180 +3433,58 @@
         <v>10000</v>
       </c>
       <c r="H14" s="22">
-        <v>15</v>
-      </c>
-      <c r="I14" s="2">
-        <v>10000</v>
-      </c>
-      <c r="J14" s="30">
-        <v>3.0000000000000001E-3</v>
-      </c>
-      <c r="K14" s="72">
+        <v>20</v>
+      </c>
+      <c r="I14" s="5">
+        <v>20000</v>
+      </c>
+      <c r="J14" s="8">
+        <v>0.03</v>
+      </c>
+      <c r="K14" s="5">
         <v>0.01</v>
       </c>
-      <c r="L14" s="54">
-        <v>0.88269550748752001</v>
-      </c>
-      <c r="M14" s="54">
-        <v>0.78737541528239197</v>
-      </c>
-      <c r="N14" s="21" t="s">
-        <v>105</v>
-      </c>
-      <c r="O14" s="41" t="s">
-        <v>106</v>
+      <c r="L14" s="91">
+        <v>0.97420965058236197</v>
+      </c>
+      <c r="M14" s="91">
+        <v>0.84053156146179397</v>
+      </c>
+      <c r="N14" s="53" t="s">
+        <v>117</v>
+      </c>
+      <c r="O14" s="62" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="15" spans="1:15">
-      <c r="B15" s="66" t="s">
-        <v>24</v>
-      </c>
-      <c r="C15" s="67" t="s">
-        <v>29</v>
-      </c>
-      <c r="D15" s="5">
-        <v>3</v>
-      </c>
-      <c r="E15" s="8">
-        <v>0.8</v>
-      </c>
-      <c r="F15" s="8">
-        <v>0.2</v>
-      </c>
-      <c r="G15" s="9">
-        <v>10000</v>
-      </c>
-      <c r="H15" s="22">
-        <v>20</v>
-      </c>
-      <c r="I15" s="5">
-        <v>10000</v>
-      </c>
-      <c r="J15" s="8">
-        <v>0.01</v>
-      </c>
-      <c r="K15" s="5">
-        <v>0.01</v>
-      </c>
-      <c r="L15" s="55">
-        <v>0.86439267886855198</v>
-      </c>
-      <c r="M15" s="55">
-        <v>0.76744186046511598</v>
-      </c>
-      <c r="N15" s="53" t="s">
-        <v>111</v>
-      </c>
-      <c r="O15" s="14" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15">
-      <c r="B16" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="C16" s="65" t="s">
-        <v>29</v>
-      </c>
-      <c r="D16" s="5">
-        <v>3</v>
-      </c>
-      <c r="E16" s="8">
-        <v>0.8</v>
-      </c>
-      <c r="F16" s="8">
-        <v>0.2</v>
-      </c>
-      <c r="G16" s="9">
-        <v>10000</v>
-      </c>
-      <c r="H16" s="22">
-        <v>20</v>
-      </c>
-      <c r="I16" s="5"/>
-      <c r="J16" s="22"/>
-      <c r="K16" s="22"/>
-      <c r="L16" s="62"/>
-      <c r="M16" s="63"/>
-      <c r="N16" s="21"/>
-      <c r="O16" s="21"/>
-    </row>
-    <row r="17" spans="2:15">
-      <c r="B17" s="12" t="s">
-        <v>67</v>
-      </c>
-      <c r="C17" s="65" t="s">
-        <v>68</v>
-      </c>
-      <c r="D17" s="5">
-        <v>3</v>
-      </c>
-      <c r="E17" s="8">
-        <v>0.8</v>
-      </c>
-      <c r="F17" s="8">
-        <v>0.2</v>
-      </c>
-      <c r="G17" s="9">
-        <v>10000</v>
-      </c>
-      <c r="H17" s="22">
-        <v>20</v>
-      </c>
-      <c r="I17" s="5"/>
-      <c r="J17" s="8"/>
-      <c r="K17" s="5"/>
-      <c r="L17" s="55"/>
-      <c r="M17" s="55"/>
-      <c r="N17" s="53"/>
-      <c r="O17" s="64"/>
-    </row>
-    <row r="18" spans="2:15" ht="15.75" thickBot="1">
-      <c r="B18" s="48" t="s">
-        <v>69</v>
-      </c>
-      <c r="C18" s="49" t="s">
-        <v>70</v>
-      </c>
-      <c r="D18" s="50">
-        <v>3</v>
-      </c>
-      <c r="E18" s="49">
-        <v>0.8</v>
-      </c>
-      <c r="F18" s="49">
-        <v>0.2</v>
-      </c>
-      <c r="G18" s="68">
-        <v>10000</v>
-      </c>
-      <c r="H18" s="70">
-        <v>20</v>
-      </c>
-      <c r="I18" s="69"/>
-      <c r="J18" s="59"/>
-      <c r="K18" s="59"/>
-      <c r="L18" s="56"/>
-      <c r="M18" s="57"/>
-      <c r="N18" s="60"/>
-      <c r="O18" s="61"/>
+      <c r="L15" s="95">
+        <v>0.965890183028286</v>
+      </c>
+      <c r="M15" s="95">
+        <v>0.84717607973421905</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="N7" r:id="rId1" xr:uid="{D22DED53-231D-4FA7-BCB0-A25A89B5065F}"/>
     <hyperlink ref="O7" r:id="rId2" xr:uid="{D864631C-3D57-4DB6-9D0E-41A56306F3FD}"/>
-    <hyperlink ref="N11" r:id="rId3" xr:uid="{3A243E82-1CB3-4D42-BD3A-33E52FF157E9}"/>
-    <hyperlink ref="O11" r:id="rId4" xr:uid="{DC027FAF-49D5-4EDF-941C-0532991EA697}"/>
-    <hyperlink ref="N9" r:id="rId5" xr:uid="{B6BE1945-F487-4886-BE4B-1F88956EF503}"/>
-    <hyperlink ref="O9" r:id="rId6" xr:uid="{9FB1C9B4-2C27-4FEB-BDDB-1A26434135B6}"/>
-    <hyperlink ref="N12" r:id="rId7" xr:uid="{F937DDF1-C004-4425-ACF7-87525BBC38F1}"/>
-    <hyperlink ref="O12" r:id="rId8" xr:uid="{2444CF7E-A702-4877-8911-CCD94F78E210}"/>
-    <hyperlink ref="N14" r:id="rId9" xr:uid="{B4CB9A64-5A41-4B25-9DA4-2A64C4DA1840}"/>
-    <hyperlink ref="O14" r:id="rId10" xr:uid="{1A041FEA-7C3B-414D-9356-E9A3B80D88A7}"/>
-    <hyperlink ref="O15" r:id="rId11" xr:uid="{B57CC596-4568-460F-AD5B-C757DE7D99F5}"/>
+    <hyperlink ref="N9" r:id="rId3" xr:uid="{3A243E82-1CB3-4D42-BD3A-33E52FF157E9}"/>
+    <hyperlink ref="O9" r:id="rId4" xr:uid="{DC027FAF-49D5-4EDF-941C-0532991EA697}"/>
+    <hyperlink ref="N8" r:id="rId5" xr:uid="{B6BE1945-F487-4886-BE4B-1F88956EF503}"/>
+    <hyperlink ref="O8" r:id="rId6" xr:uid="{9FB1C9B4-2C27-4FEB-BDDB-1A26434135B6}"/>
+    <hyperlink ref="N10" r:id="rId7" xr:uid="{F937DDF1-C004-4425-ACF7-87525BBC38F1}"/>
+    <hyperlink ref="O10" r:id="rId8" xr:uid="{2444CF7E-A702-4877-8911-CCD94F78E210}"/>
+    <hyperlink ref="N11" r:id="rId9" xr:uid="{B4CB9A64-5A41-4B25-9DA4-2A64C4DA1840}"/>
+    <hyperlink ref="O11" r:id="rId10" xr:uid="{1A041FEA-7C3B-414D-9356-E9A3B80D88A7}"/>
+    <hyperlink ref="O12" r:id="rId11" xr:uid="{B57CC596-4568-460F-AD5B-C757DE7D99F5}"/>
+    <hyperlink ref="N13" r:id="rId12" xr:uid="{4FF4CC27-ABAD-442E-9F16-B667801EA134}"/>
+    <hyperlink ref="O13" r:id="rId13" xr:uid="{04C6CC64-B085-43C6-9B85-A80098D9FDA3}"/>
+    <hyperlink ref="N14" r:id="rId14" xr:uid="{0A56BBE2-84BB-4709-BF41-1A06D44C5905}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId15"/>
 </worksheet>
 </file>
 
@@ -3658,51 +3510,51 @@
     <row r="4" spans="2:14" ht="15.75" thickBot="1"/>
     <row r="5" spans="2:14" ht="15.75" thickBot="1">
       <c r="K5" s="92" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="L5" s="93"/>
       <c r="M5" s="93"/>
       <c r="N5" s="94"/>
     </row>
     <row r="6" spans="2:14" ht="15.75" thickBot="1">
-      <c r="B6" s="80" t="s">
-        <v>76</v>
-      </c>
-      <c r="C6" s="81" t="s">
-        <v>75</v>
-      </c>
-      <c r="D6" s="82" t="s">
-        <v>77</v>
-      </c>
-      <c r="E6" s="82" t="s">
-        <v>78</v>
-      </c>
-      <c r="F6" s="82" t="s">
+      <c r="B6" s="74" t="s">
+        <v>72</v>
+      </c>
+      <c r="C6" s="75" t="s">
+        <v>71</v>
+      </c>
+      <c r="D6" s="76" t="s">
+        <v>73</v>
+      </c>
+      <c r="E6" s="76" t="s">
+        <v>74</v>
+      </c>
+      <c r="F6" s="76" t="s">
         <v>1</v>
       </c>
-      <c r="G6" s="82" t="s">
-        <v>100</v>
-      </c>
-      <c r="H6" s="82" t="s">
+      <c r="G6" s="76" t="s">
+        <v>96</v>
+      </c>
+      <c r="H6" s="76" t="s">
         <v>4</v>
       </c>
-      <c r="I6" s="83" t="s">
+      <c r="I6" s="77" t="s">
         <v>43</v>
       </c>
-      <c r="J6" s="84" t="s">
+      <c r="J6" s="78" t="s">
         <v>42</v>
       </c>
-      <c r="K6" s="91" t="s">
+      <c r="K6" s="85" t="s">
+        <v>87</v>
+      </c>
+      <c r="L6" s="82" t="s">
+        <v>84</v>
+      </c>
+      <c r="M6" s="82" t="s">
+        <v>85</v>
+      </c>
+      <c r="N6" s="83" t="s">
         <v>91</v>
-      </c>
-      <c r="L6" s="88" t="s">
-        <v>88</v>
-      </c>
-      <c r="M6" s="88" t="s">
-        <v>89</v>
-      </c>
-      <c r="N6" s="89" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="7" spans="2:14">
@@ -3722,7 +3574,7 @@
         <v>0.2</v>
       </c>
       <c r="G7" s="24" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="H7" s="24">
         <v>20000</v>
@@ -3730,20 +3582,20 @@
       <c r="I7" s="42">
         <v>0.99750415973377704</v>
       </c>
-      <c r="J7" s="78">
+      <c r="J7" s="72">
         <v>0.77076411960132896</v>
       </c>
-      <c r="K7" s="95" t="s">
+      <c r="K7" s="86" t="s">
+        <v>86</v>
+      </c>
+      <c r="L7" s="81" t="s">
+        <v>89</v>
+      </c>
+      <c r="M7" s="81" t="s">
+        <v>113</v>
+      </c>
+      <c r="N7" s="79" t="s">
         <v>90</v>
-      </c>
-      <c r="L7" s="87" t="s">
-        <v>93</v>
-      </c>
-      <c r="M7" s="87" t="s">
-        <v>117</v>
-      </c>
-      <c r="N7" s="85" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="8" spans="2:14">
@@ -3763,7 +3615,7 @@
         <v>0.3</v>
       </c>
       <c r="G8" s="8" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="H8" s="8">
         <v>20000</v>
@@ -3771,20 +3623,20 @@
       <c r="I8" s="54">
         <v>0.99904942965779397</v>
       </c>
-      <c r="J8" s="79">
+      <c r="J8" s="73">
         <v>0.77827050997782699</v>
       </c>
-      <c r="K8" s="74" t="s">
-        <v>99</v>
-      </c>
-      <c r="L8" s="74" t="s">
-        <v>98</v>
-      </c>
-      <c r="M8" s="74" t="s">
-        <v>97</v>
-      </c>
-      <c r="N8" s="75" t="s">
-        <v>96</v>
+      <c r="K8" s="68" t="s">
+        <v>95</v>
+      </c>
+      <c r="L8" s="68" t="s">
+        <v>94</v>
+      </c>
+      <c r="M8" s="68" t="s">
+        <v>93</v>
+      </c>
+      <c r="N8" s="69" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="9" spans="2:14" ht="15.75" thickBot="1">
@@ -3809,87 +3661,87 @@
       <c r="H9" s="16">
         <v>20000</v>
       </c>
-      <c r="I9" s="76">
+      <c r="I9" s="70">
         <v>1</v>
       </c>
-      <c r="J9" s="98">
+      <c r="J9" s="89">
         <v>0.79734219269103002</v>
       </c>
-      <c r="K9" s="86" t="s">
-        <v>104</v>
-      </c>
-      <c r="L9" s="86" t="s">
-        <v>118</v>
-      </c>
-      <c r="M9" s="99" t="s">
-        <v>103</v>
-      </c>
-      <c r="N9" s="77" t="s">
-        <v>102</v>
+      <c r="K9" s="80" t="s">
+        <v>100</v>
+      </c>
+      <c r="L9" s="80" t="s">
+        <v>114</v>
+      </c>
+      <c r="M9" s="90" t="s">
+        <v>99</v>
+      </c>
+      <c r="N9" s="71" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="10" spans="2:14" ht="15.75" thickBot="1">
-      <c r="B10" s="96"/>
-      <c r="C10" s="97"/>
+      <c r="B10" s="87"/>
+      <c r="C10" s="88"/>
       <c r="D10" s="7"/>
-      <c r="E10" s="97"/>
-      <c r="F10" s="97"/>
-      <c r="G10" s="97"/>
-      <c r="H10" s="97"/>
-      <c r="I10" s="73"/>
-      <c r="J10" s="73"/>
-      <c r="K10" s="90"/>
-      <c r="L10" s="90"/>
-      <c r="M10" s="90"/>
-      <c r="N10" s="90"/>
+      <c r="E10" s="88"/>
+      <c r="F10" s="88"/>
+      <c r="G10" s="88"/>
+      <c r="H10" s="88"/>
+      <c r="I10" s="67"/>
+      <c r="J10" s="67"/>
+      <c r="K10" s="84"/>
+      <c r="L10" s="84"/>
+      <c r="M10" s="84"/>
+      <c r="N10" s="84"/>
     </row>
     <row r="11" spans="2:14" ht="15.75" thickBot="1">
       <c r="K11" s="92" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="L11" s="93"/>
       <c r="M11" s="93"/>
       <c r="N11" s="94"/>
     </row>
     <row r="12" spans="2:14" ht="15.75" thickBot="1">
-      <c r="B12" s="80" t="s">
-        <v>76</v>
-      </c>
-      <c r="C12" s="81" t="s">
-        <v>75</v>
-      </c>
-      <c r="D12" s="82" t="s">
-        <v>77</v>
-      </c>
-      <c r="E12" s="82" t="s">
-        <v>78</v>
-      </c>
-      <c r="F12" s="82" t="s">
+      <c r="B12" s="74" t="s">
+        <v>72</v>
+      </c>
+      <c r="C12" s="75" t="s">
+        <v>71</v>
+      </c>
+      <c r="D12" s="76" t="s">
+        <v>73</v>
+      </c>
+      <c r="E12" s="76" t="s">
+        <v>74</v>
+      </c>
+      <c r="F12" s="76" t="s">
         <v>1</v>
       </c>
-      <c r="G12" s="82" t="s">
-        <v>100</v>
-      </c>
-      <c r="H12" s="82" t="s">
+      <c r="G12" s="76" t="s">
+        <v>96</v>
+      </c>
+      <c r="H12" s="76" t="s">
         <v>4</v>
       </c>
-      <c r="I12" s="83" t="s">
+      <c r="I12" s="77" t="s">
         <v>43</v>
       </c>
-      <c r="J12" s="84" t="s">
+      <c r="J12" s="78" t="s">
         <v>42</v>
       </c>
-      <c r="K12" s="91" t="s">
+      <c r="K12" s="85" t="s">
+        <v>87</v>
+      </c>
+      <c r="L12" s="82" t="s">
+        <v>84</v>
+      </c>
+      <c r="M12" s="82" t="s">
+        <v>85</v>
+      </c>
+      <c r="N12" s="83" t="s">
         <v>91</v>
-      </c>
-      <c r="L12" s="88" t="s">
-        <v>88</v>
-      </c>
-      <c r="M12" s="88" t="s">
-        <v>89</v>
-      </c>
-      <c r="N12" s="89" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="13" spans="2:14" ht="15.75" thickBot="1">
@@ -3909,28 +3761,28 @@
         <v>0.2</v>
       </c>
       <c r="G13" s="24" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="H13" s="24">
         <v>20000</v>
       </c>
-      <c r="I13" s="76">
+      <c r="I13" s="70">
         <v>1</v>
       </c>
-      <c r="J13" s="100">
+      <c r="J13" s="91">
         <v>0.76744186046511598</v>
       </c>
-      <c r="K13" s="95" t="s">
-        <v>115</v>
-      </c>
-      <c r="L13" s="87" t="s">
-        <v>114</v>
-      </c>
-      <c r="M13" s="87" t="s">
-        <v>113</v>
-      </c>
-      <c r="N13" s="85" t="s">
-        <v>116</v>
+      <c r="K13" s="86" t="s">
+        <v>111</v>
+      </c>
+      <c r="L13" s="81" t="s">
+        <v>110</v>
+      </c>
+      <c r="M13" s="81" t="s">
+        <v>109</v>
+      </c>
+      <c r="N13" s="79" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="14" spans="2:14" ht="15.75" thickBot="1">
@@ -3950,28 +3802,28 @@
         <v>0.3</v>
       </c>
       <c r="G14" s="8" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="H14" s="8">
         <v>20000</v>
       </c>
-      <c r="I14" s="76">
+      <c r="I14" s="70">
         <v>1</v>
       </c>
-      <c r="J14" s="79">
+      <c r="J14" s="73">
         <v>0.76940133037694003</v>
       </c>
-      <c r="K14" s="74" t="s">
-        <v>99</v>
-      </c>
-      <c r="L14" s="74" t="s">
-        <v>98</v>
-      </c>
-      <c r="M14" s="74" t="s">
-        <v>97</v>
-      </c>
-      <c r="N14" s="75" t="s">
-        <v>96</v>
+      <c r="K14" s="68" t="s">
+        <v>95</v>
+      </c>
+      <c r="L14" s="68" t="s">
+        <v>94</v>
+      </c>
+      <c r="M14" s="68" t="s">
+        <v>93</v>
+      </c>
+      <c r="N14" s="69" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="15" spans="2:14" ht="15.75" thickBot="1">
@@ -3996,42 +3848,42 @@
       <c r="H15" s="16">
         <v>20000</v>
       </c>
-      <c r="I15" s="76">
+      <c r="I15" s="70">
         <v>1</v>
       </c>
-      <c r="J15" s="98">
+      <c r="J15" s="89">
         <v>0.77408637873754105</v>
       </c>
-      <c r="K15" s="86" t="s">
-        <v>107</v>
-      </c>
-      <c r="L15" s="86" t="s">
-        <v>108</v>
-      </c>
-      <c r="M15" s="99" t="s">
-        <v>109</v>
-      </c>
-      <c r="N15" s="77" t="s">
-        <v>110</v>
+      <c r="K15" s="80" t="s">
+        <v>103</v>
+      </c>
+      <c r="L15" s="80" t="s">
+        <v>104</v>
+      </c>
+      <c r="M15" s="90" t="s">
+        <v>105</v>
+      </c>
+      <c r="N15" s="71" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="16" spans="2:14">
-      <c r="B16" s="96"/>
-      <c r="C16" s="97"/>
+      <c r="B16" s="87"/>
+      <c r="C16" s="88"/>
       <c r="D16" s="7"/>
-      <c r="E16" s="97"/>
-      <c r="F16" s="97"/>
-      <c r="G16" s="97"/>
-      <c r="H16" s="97"/>
-      <c r="I16" s="73"/>
-      <c r="J16" s="90"/>
-      <c r="K16" s="90"/>
-      <c r="L16" s="90"/>
-      <c r="M16" s="90"/>
-      <c r="N16" s="90"/>
+      <c r="E16" s="88"/>
+      <c r="F16" s="88"/>
+      <c r="G16" s="88"/>
+      <c r="H16" s="88"/>
+      <c r="I16" s="67"/>
+      <c r="J16" s="84"/>
+      <c r="K16" s="84"/>
+      <c r="L16" s="84"/>
+      <c r="M16" s="84"/>
+      <c r="N16" s="84"/>
     </row>
     <row r="17" spans="9:9">
-      <c r="I17" s="73"/>
+      <c r="I17" s="67"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>